<commit_message>
update report sarana bantu pemandu
</commit_message>
<xml_diff>
--- a/report/Report-Inspection-Sarana Bantu Pemanduan 1.xlsx
+++ b/report/Report-Inspection-Sarana Bantu Pemanduan 1.xlsx
@@ -256,9 +256,6 @@
   </si>
   <si>
     <t>${table:operator.nama}</t>
-  </si>
-  <si>
-    <t>${table:operator.jabatan}</t>
   </si>
   <si>
     <t>B. DOKUMEN PERALATAN KOMUNIKASI</t>
@@ -1129,12 +1126,15 @@
   <si>
     <t>${kkm_jabatan}</t>
   </si>
+  <si>
+    <t>Radio Operator</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1217,6 +1217,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1409,7 +1415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1500,56 +1506,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1563,6 +1530,46 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1845,8 +1852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1862,15 +1869,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
       <c r="H1" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -1878,7 +1885,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -1886,7 +1893,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -1894,19 +1901,19 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
@@ -1928,29 +1935,29 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56" t="s">
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="56"/>
+      <c r="H12" s="55"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="56"/>
-      <c r="B13" s="56"/>
-      <c r="C13" s="56"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
       <c r="D13" s="4" t="s">
         <v>12</v>
       </c>
@@ -1960,56 +1967,56 @@
       <c r="F13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
     </row>
     <row r="14" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>1</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C14" s="50" t="s">
         <v>289</v>
       </c>
-      <c r="C14" s="50" t="s">
+      <c r="D14" s="51" t="s">
         <v>290</v>
       </c>
-      <c r="D14" s="51" t="s">
+      <c r="E14" s="52" t="s">
         <v>291</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="F14" s="52" t="s">
         <v>292</v>
       </c>
-      <c r="F14" s="52" t="s">
+      <c r="G14" s="54" t="s">
         <v>293</v>
       </c>
-      <c r="G14" s="57" t="s">
-        <v>294</v>
-      </c>
-      <c r="H14" s="57"/>
+      <c r="H14" s="54"/>
     </row>
     <row r="15" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>2</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>307</v>
+      </c>
+      <c r="D15" s="51" t="s">
         <v>303</v>
       </c>
-      <c r="C15" s="53" t="s">
-        <v>308</v>
-      </c>
-      <c r="D15" s="51" t="s">
+      <c r="E15" s="52" t="s">
         <v>304</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="F15" s="52" t="s">
         <v>305</v>
       </c>
-      <c r="F15" s="52" t="s">
+      <c r="G15" s="54" t="s">
         <v>306</v>
       </c>
-      <c r="G15" s="57" t="s">
-        <v>307</v>
-      </c>
-      <c r="H15" s="57"/>
+      <c r="H15" s="54"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
@@ -2043,21 +2050,21 @@
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="56" t="s">
+      <c r="C19" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
     </row>
     <row r="20" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="56"/>
-      <c r="B20" s="56"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="4" t="s">
         <v>12</v>
       </c>
@@ -2316,15 +2323,15 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="54" t="s">
+      <c r="A41" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="54"/>
-      <c r="C41" s="54"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="54"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="54"/>
+      <c r="B41" s="56"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="56"/>
+      <c r="F41" s="56"/>
+      <c r="G41" s="56"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
@@ -2335,28 +2342,28 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="56" t="s">
+      <c r="A44" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="56" t="s">
+      <c r="B44" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="56" t="s">
+      <c r="C44" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="D44" s="56" t="s">
+      <c r="D44" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="56"/>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56" t="s">
+      <c r="E44" s="55"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="55" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="56"/>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
+      <c r="A45" s="55"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="55"/>
       <c r="D45" s="4" t="s">
         <v>12</v>
       </c>
@@ -2366,7 +2373,7 @@
       <c r="F45" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G45" s="56"/>
+      <c r="G45" s="55"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="17" t="s">
@@ -2375,25 +2382,25 @@
       <c r="B46" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C46" s="17" t="s">
-        <v>76</v>
+      <c r="C46" s="75" t="s">
+        <v>308</v>
       </c>
       <c r="D46" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="E46" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="F46" s="12" t="s">
         <v>296</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="G46" s="17" t="s">
         <v>297</v>
-      </c>
-      <c r="G46" s="17" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -2410,7 +2417,7 @@
         <v>18</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>12</v>
@@ -2427,30 +2434,30 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="C50" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C50" s="17" t="s">
-        <v>81</v>
-      </c>
       <c r="D50" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="E50" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="F50" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="G50" s="17" t="s">
         <v>301</v>
-      </c>
-      <c r="G50" s="17" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B52" s="19"/>
       <c r="C52" s="19"/>
@@ -2505,10 +2512,10 @@
       <c r="G57" s="24"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" s="54" t="s">
-        <v>83</v>
-      </c>
-      <c r="B59" s="54"/>
+      <c r="A59" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="B59" s="56"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="3"/>
@@ -2527,13 +2534,21 @@
       <c r="B63" s="25"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64" s="55" t="s">
-        <v>84</v>
-      </c>
-      <c r="B64" s="55"/>
+      <c r="A64" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="B64" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="G44:G45"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
@@ -2546,14 +2561,6 @@
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="G12:H13"/>
     <mergeCell ref="G15:H15"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A41:G41"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="G44:G45"/>
   </mergeCells>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" scale="80" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2577,27 +2584,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="71" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
+      <c r="A1" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -2605,7 +2612,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -2613,47 +2620,47 @@
         <v>3</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="72" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
+      <c r="C8" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B9" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="28" t="s">
         <v>89</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>90</v>
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
       <c r="H9" s="28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I9" s="29"/>
       <c r="J9" s="29"/>
@@ -2662,17 +2669,17 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B10" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="28" t="s">
         <v>92</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>93</v>
       </c>
       <c r="D10" s="29"/>
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
       <c r="H10" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I10" s="29"/>
       <c r="J10" s="29"/>
@@ -2681,17 +2688,17 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B11" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="28" t="s">
         <v>95</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>96</v>
       </c>
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
       <c r="H11" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I11" s="29"/>
       <c r="J11" s="29"/>
@@ -2700,17 +2707,17 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B12" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="28" t="s">
         <v>98</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>99</v>
       </c>
       <c r="D12" s="29"/>
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
       <c r="H12" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I12" s="29"/>
       <c r="J12" s="29"/>
@@ -2719,17 +2726,17 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B13" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="28" t="s">
         <v>101</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>102</v>
       </c>
       <c r="D13" s="29"/>
       <c r="E13" s="29"/>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
       <c r="H13" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I13" s="29"/>
       <c r="J13" s="29"/>
@@ -2738,17 +2745,17 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B14" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="28" t="s">
         <v>104</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>105</v>
       </c>
       <c r="D14" s="29"/>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
       <c r="H14" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I14" s="29"/>
       <c r="J14" s="29"/>
@@ -2757,17 +2764,17 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B15" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="28" t="s">
         <v>107</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>108</v>
       </c>
       <c r="D15" s="29"/>
       <c r="E15" s="29"/>
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
       <c r="H15" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I15" s="29"/>
       <c r="J15" s="29"/>
@@ -2776,35 +2783,35 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B18" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="72" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
-      <c r="L18" s="72"/>
+      <c r="C18" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B19" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D19" s="29"/>
       <c r="E19" s="29"/>
@@ -2818,17 +2825,17 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B20" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D20" s="29"/>
       <c r="E20" s="29"/>
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
       <c r="H20" s="28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I20" s="29"/>
       <c r="J20" s="29"/>
@@ -2837,17 +2844,17 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B21" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D21" s="29"/>
       <c r="E21" s="29"/>
       <c r="F21" s="29"/>
       <c r="G21" s="29"/>
       <c r="H21" s="28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I21" s="29"/>
       <c r="J21" s="29"/>
@@ -2856,10 +2863,10 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B22" s="28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D22" s="29"/>
       <c r="E22" s="29"/>
@@ -2873,17 +2880,17 @@
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" s="73" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="33" t="s">
         <v>118</v>
-      </c>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="33" t="s">
-        <v>119</v>
       </c>
       <c r="I23" s="19"/>
       <c r="J23" s="19"/>
@@ -2892,11 +2899,11 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B24" s="22"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
       <c r="H24" s="34"/>
       <c r="I24" s="23"/>
       <c r="J24" s="23"/>
@@ -2905,125 +2912,125 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B26" s="3" t="s">
+    </row>
+    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="55" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="56" t="s">
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56" t="s">
+      <c r="G27" s="55"/>
+      <c r="H27" s="55"/>
+      <c r="I27" s="55"/>
+      <c r="J27" s="61" t="s">
         <v>123</v>
       </c>
-      <c r="G27" s="56"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="56"/>
-      <c r="J27" s="74" t="s">
+      <c r="K27" s="61"/>
+      <c r="L27" s="61"/>
+    </row>
+    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="55"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="K27" s="74"/>
-      <c r="L27" s="74"/>
-    </row>
-    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56" t="s">
+      <c r="G28" s="55"/>
+      <c r="H28" s="61" t="s">
         <v>125</v>
       </c>
-      <c r="G28" s="56"/>
-      <c r="H28" s="74" t="s">
-        <v>126</v>
-      </c>
-      <c r="I28" s="74"/>
-      <c r="J28" s="74"/>
-      <c r="K28" s="74"/>
-      <c r="L28" s="74"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="61"/>
+      <c r="L28" s="61"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="74"/>
-      <c r="K29" s="74"/>
-      <c r="L29" s="74"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
+      <c r="L29" s="61"/>
     </row>
     <row r="30" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="35">
         <v>1</v>
       </c>
-      <c r="C30" s="63" t="s">
+      <c r="C30" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" s="62"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="63" t="s">
         <v>127</v>
       </c>
-      <c r="D30" s="63"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="69" t="s">
+      <c r="G30" s="63"/>
+      <c r="H30" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="G30" s="69"/>
-      <c r="H30" s="69" t="s">
-        <v>129</v>
-      </c>
-      <c r="I30" s="69"/>
-      <c r="J30" s="65"/>
-      <c r="K30" s="65"/>
-      <c r="L30" s="65"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="64"/>
+      <c r="K30" s="64"/>
+      <c r="L30" s="64"/>
     </row>
     <row r="31" spans="1:12" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="35">
         <v>2</v>
       </c>
-      <c r="C31" s="63" t="s">
+      <c r="C31" s="62" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="69" t="s">
+      <c r="G31" s="63"/>
+      <c r="H31" s="63" t="s">
         <v>131</v>
       </c>
-      <c r="G31" s="69"/>
-      <c r="H31" s="69" t="s">
-        <v>132</v>
-      </c>
-      <c r="I31" s="69"/>
-      <c r="J31" s="70"/>
-      <c r="K31" s="70"/>
-      <c r="L31" s="70"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="65"/>
+      <c r="K31" s="65"/>
+      <c r="L31" s="65"/>
     </row>
     <row r="32" spans="1:12" ht="71" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="35">
         <v>3</v>
       </c>
-      <c r="C32" s="63" t="s">
+      <c r="C32" s="62" t="s">
+        <v>132</v>
+      </c>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="64" t="s">
+      <c r="G32" s="66"/>
+      <c r="H32" s="66" t="s">
         <v>134</v>
       </c>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64" t="s">
-        <v>135</v>
-      </c>
-      <c r="I32" s="64"/>
-      <c r="J32" s="65"/>
-      <c r="K32" s="65"/>
-      <c r="L32" s="65"/>
+      <c r="I32" s="66"/>
+      <c r="J32" s="64"/>
+      <c r="K32" s="64"/>
+      <c r="L32" s="64"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B33" s="6"/>
@@ -3040,77 +3047,77 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B35" s="3" t="s">
+    </row>
+    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="67" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" s="67"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="68" t="s">
+        <v>122</v>
+      </c>
+      <c r="G36" s="68"/>
+      <c r="H36" s="68"/>
+      <c r="I36" s="68"/>
+      <c r="J36" s="69" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="66" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="66" t="s">
-        <v>122</v>
-      </c>
-      <c r="D36" s="66"/>
-      <c r="E36" s="66"/>
-      <c r="F36" s="67" t="s">
-        <v>123</v>
-      </c>
-      <c r="G36" s="67"/>
-      <c r="H36" s="67"/>
-      <c r="I36" s="67"/>
-      <c r="J36" s="68" t="s">
+      <c r="K36" s="69"/>
+      <c r="L36" s="69"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B37" s="67"/>
+      <c r="C37" s="67"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="68" t="s">
         <v>138</v>
       </c>
-      <c r="K36" s="68"/>
-      <c r="L36" s="68"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B37" s="66"/>
-      <c r="C37" s="66"/>
-      <c r="D37" s="66"/>
-      <c r="E37" s="66"/>
-      <c r="F37" s="67" t="s">
+      <c r="G37" s="68"/>
+      <c r="H37" s="68" t="s">
         <v>139</v>
       </c>
-      <c r="G37" s="67"/>
-      <c r="H37" s="67" t="s">
+      <c r="I37" s="68"/>
+      <c r="J37" s="69"/>
+      <c r="K37" s="69"/>
+      <c r="L37" s="69"/>
+    </row>
+    <row r="38" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="B38" s="67"/>
+      <c r="C38" s="67"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="38" t="s">
         <v>140</v>
-      </c>
-      <c r="I37" s="67"/>
-      <c r="J37" s="68"/>
-      <c r="K37" s="68"/>
-      <c r="L37" s="68"/>
-    </row>
-    <row r="38" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="B38" s="66"/>
-      <c r="C38" s="66"/>
-      <c r="D38" s="66"/>
-      <c r="E38" s="66"/>
-      <c r="F38" s="38" t="s">
-        <v>141</v>
       </c>
       <c r="G38" s="38" t="s">
         <v>14</v>
       </c>
       <c r="H38" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="I38" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="I38" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="J38" s="68"/>
-      <c r="K38" s="68"/>
-      <c r="L38" s="68"/>
+      <c r="J38" s="69"/>
+      <c r="K38" s="69"/>
+      <c r="L38" s="69"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B39" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" s="40" t="s">
         <v>144</v>
-      </c>
-      <c r="C39" s="40" t="s">
-        <v>145</v>
       </c>
       <c r="D39" s="29"/>
       <c r="E39" s="29"/>
@@ -3127,7 +3134,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D40" s="29"/>
       <c r="E40" s="30"/>
@@ -3136,13 +3143,13 @@
         <v></v>
       </c>
       <c r="G40" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="H40" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="H40" s="42" t="s">
+      <c r="I40" s="42" t="s">
         <v>148</v>
-      </c>
-      <c r="I40" s="42" t="s">
-        <v>149</v>
       </c>
       <c r="J40" s="43"/>
       <c r="K40" s="29"/>
@@ -3153,7 +3160,7 @@
         <v>2</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D41" s="29"/>
       <c r="E41" s="30"/>
@@ -3162,13 +3169,13 @@
         <v></v>
       </c>
       <c r="G41" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="H41" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="H41" s="42" t="s">
+      <c r="I41" s="42" t="s">
         <v>152</v>
-      </c>
-      <c r="I41" s="42" t="s">
-        <v>153</v>
       </c>
       <c r="J41" s="43"/>
       <c r="K41" s="29"/>
@@ -3179,7 +3186,7 @@
         <v>3</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D42" s="29"/>
       <c r="E42" s="30"/>
@@ -3188,13 +3195,13 @@
         <v></v>
       </c>
       <c r="G42" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="H42" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="H42" s="42" t="s">
+      <c r="I42" s="42" t="s">
         <v>156</v>
-      </c>
-      <c r="I42" s="42" t="s">
-        <v>157</v>
       </c>
       <c r="J42" s="43"/>
       <c r="K42" s="29"/>
@@ -3205,7 +3212,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="30"/>
@@ -3214,13 +3221,13 @@
         <v></v>
       </c>
       <c r="G43" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="H43" s="42" t="s">
         <v>159</v>
       </c>
-      <c r="H43" s="42" t="s">
+      <c r="I43" s="42" t="s">
         <v>160</v>
-      </c>
-      <c r="I43" s="42" t="s">
-        <v>161</v>
       </c>
       <c r="J43" s="43"/>
       <c r="K43" s="29"/>
@@ -3231,7 +3238,7 @@
         <v>5</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D44" s="29"/>
       <c r="E44" s="30"/>
@@ -3240,13 +3247,13 @@
         <v></v>
       </c>
       <c r="G44" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="H44" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="H44" s="42" t="s">
+      <c r="I44" s="42" t="s">
         <v>164</v>
-      </c>
-      <c r="I44" s="42" t="s">
-        <v>165</v>
       </c>
       <c r="J44" s="43"/>
       <c r="K44" s="29"/>
@@ -3254,10 +3261,10 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B45" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="C45" s="40" t="s">
         <v>166</v>
-      </c>
-      <c r="C45" s="40" t="s">
-        <v>167</v>
       </c>
       <c r="D45" s="29"/>
       <c r="E45" s="29"/>
@@ -3274,7 +3281,7 @@
         <v>1</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D46" s="29"/>
       <c r="E46" s="30"/>
@@ -3283,13 +3290,13 @@
         <v></v>
       </c>
       <c r="G46" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="H46" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="H46" s="42" t="s">
+      <c r="I46" s="44" t="s">
         <v>170</v>
-      </c>
-      <c r="I46" s="44" t="s">
-        <v>171</v>
       </c>
       <c r="J46" s="43"/>
       <c r="K46" s="29"/>
@@ -3300,7 +3307,7 @@
         <v>2</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D47" s="29"/>
       <c r="E47" s="30"/>
@@ -3309,13 +3316,13 @@
         <v></v>
       </c>
       <c r="G47" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="H47" s="44" t="s">
         <v>173</v>
       </c>
-      <c r="H47" s="44" t="s">
+      <c r="I47" s="44" t="s">
         <v>174</v>
-      </c>
-      <c r="I47" s="44" t="s">
-        <v>175</v>
       </c>
       <c r="J47" s="43"/>
       <c r="K47" s="29"/>
@@ -3326,7 +3333,7 @@
         <v>3</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D48" s="29"/>
       <c r="E48" s="30"/>
@@ -3335,13 +3342,13 @@
         <v></v>
       </c>
       <c r="G48" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="H48" s="44" t="s">
         <v>177</v>
       </c>
-      <c r="H48" s="44" t="s">
+      <c r="I48" s="44" t="s">
         <v>178</v>
-      </c>
-      <c r="I48" s="44" t="s">
-        <v>179</v>
       </c>
       <c r="J48" s="43"/>
       <c r="K48" s="29"/>
@@ -3352,7 +3359,7 @@
         <v>4</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D49" s="29"/>
       <c r="E49" s="30"/>
@@ -3361,13 +3368,13 @@
         <v></v>
       </c>
       <c r="G49" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="H49" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="H49" s="44" t="s">
+      <c r="I49" s="44" t="s">
         <v>182</v>
-      </c>
-      <c r="I49" s="44" t="s">
-        <v>183</v>
       </c>
       <c r="J49" s="43"/>
       <c r="K49" s="29"/>
@@ -3378,7 +3385,7 @@
         <v>5</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D50" s="29"/>
       <c r="E50" s="30"/>
@@ -3387,13 +3394,13 @@
         <v></v>
       </c>
       <c r="G50" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="H50" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="H50" s="42" t="s">
+      <c r="I50" s="44" t="s">
         <v>186</v>
-      </c>
-      <c r="I50" s="44" t="s">
-        <v>187</v>
       </c>
       <c r="J50" s="43"/>
       <c r="K50" s="29"/>
@@ -3404,7 +3411,7 @@
         <v>6</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D51" s="29"/>
       <c r="E51" s="30"/>
@@ -3413,13 +3420,13 @@
         <v></v>
       </c>
       <c r="G51" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="H51" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="H51" s="42" t="s">
+      <c r="I51" s="44" t="s">
         <v>190</v>
-      </c>
-      <c r="I51" s="44" t="s">
-        <v>191</v>
       </c>
       <c r="J51" s="43"/>
       <c r="K51" s="29"/>
@@ -3430,7 +3437,7 @@
         <v>7</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D52" s="29"/>
       <c r="E52" s="30"/>
@@ -3439,13 +3446,13 @@
         <v></v>
       </c>
       <c r="G52" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="H52" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="H52" s="42" t="s">
+      <c r="I52" s="44" t="s">
         <v>194</v>
-      </c>
-      <c r="I52" s="44" t="s">
-        <v>195</v>
       </c>
       <c r="J52" s="43"/>
       <c r="K52" s="29"/>
@@ -3456,7 +3463,7 @@
         <v>8</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D53" s="29"/>
       <c r="E53" s="30"/>
@@ -3465,13 +3472,13 @@
         <v></v>
       </c>
       <c r="G53" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="H53" s="44" t="s">
         <v>197</v>
       </c>
-      <c r="H53" s="44" t="s">
+      <c r="I53" s="44" t="s">
         <v>198</v>
-      </c>
-      <c r="I53" s="44" t="s">
-        <v>199</v>
       </c>
       <c r="J53" s="28"/>
       <c r="K53" s="29"/>
@@ -3492,10 +3499,10 @@
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B55" s="39" t="s">
+        <v>199</v>
+      </c>
+      <c r="C55" s="40" t="s">
         <v>200</v>
-      </c>
-      <c r="C55" s="40" t="s">
-        <v>201</v>
       </c>
       <c r="D55" s="29"/>
       <c r="E55" s="29"/>
@@ -3512,7 +3519,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D56" s="29"/>
       <c r="E56" s="30"/>
@@ -3521,13 +3528,13 @@
         <v></v>
       </c>
       <c r="G56" s="44" t="s">
+        <v>202</v>
+      </c>
+      <c r="H56" s="44" t="s">
         <v>203</v>
       </c>
-      <c r="H56" s="44" t="s">
+      <c r="I56" s="44" t="s">
         <v>204</v>
-      </c>
-      <c r="I56" s="44" t="s">
-        <v>205</v>
       </c>
       <c r="J56" s="43"/>
       <c r="K56" s="29"/>
@@ -3538,7 +3545,7 @@
         <v>2</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D57" s="29"/>
       <c r="E57" s="30"/>
@@ -3547,13 +3554,13 @@
         <v></v>
       </c>
       <c r="G57" s="44" t="s">
+        <v>206</v>
+      </c>
+      <c r="H57" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="H57" s="44" t="s">
+      <c r="I57" s="44" t="s">
         <v>208</v>
-      </c>
-      <c r="I57" s="44" t="s">
-        <v>209</v>
       </c>
       <c r="J57" s="43"/>
       <c r="K57" s="29"/>
@@ -3564,7 +3571,7 @@
         <v>3</v>
       </c>
       <c r="C58" s="45" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D58" s="29"/>
       <c r="E58" s="30"/>
@@ -3573,13 +3580,13 @@
         <v></v>
       </c>
       <c r="G58" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="H58" s="44" t="s">
         <v>211</v>
       </c>
-      <c r="H58" s="44" t="s">
+      <c r="I58" s="44" t="s">
         <v>212</v>
-      </c>
-      <c r="I58" s="44" t="s">
-        <v>213</v>
       </c>
       <c r="J58" s="43"/>
       <c r="K58" s="29"/>
@@ -3590,7 +3597,7 @@
         <v>4</v>
       </c>
       <c r="C59" s="45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="30"/>
@@ -3599,13 +3606,13 @@
         <v></v>
       </c>
       <c r="G59" s="44" t="s">
+        <v>214</v>
+      </c>
+      <c r="H59" s="44" t="s">
         <v>215</v>
       </c>
-      <c r="H59" s="44" t="s">
+      <c r="I59" s="44" t="s">
         <v>216</v>
-      </c>
-      <c r="I59" s="44" t="s">
-        <v>217</v>
       </c>
       <c r="J59" s="43"/>
       <c r="K59" s="29"/>
@@ -3616,7 +3623,7 @@
         <v>5</v>
       </c>
       <c r="C60" s="46" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D60" s="29"/>
       <c r="E60" s="30"/>
@@ -3625,13 +3632,13 @@
         <v></v>
       </c>
       <c r="G60" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="H60" s="44" t="s">
         <v>219</v>
       </c>
-      <c r="H60" s="44" t="s">
+      <c r="I60" s="44" t="s">
         <v>220</v>
-      </c>
-      <c r="I60" s="44" t="s">
-        <v>221</v>
       </c>
       <c r="J60" s="43"/>
       <c r="K60" s="29"/>
@@ -3642,7 +3649,7 @@
         <v>6</v>
       </c>
       <c r="C61" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D61" s="29"/>
       <c r="E61" s="30"/>
@@ -3651,13 +3658,13 @@
         <v></v>
       </c>
       <c r="G61" s="44" t="s">
+        <v>222</v>
+      </c>
+      <c r="H61" s="44" t="s">
         <v>223</v>
       </c>
-      <c r="H61" s="44" t="s">
+      <c r="I61" s="44" t="s">
         <v>224</v>
-      </c>
-      <c r="I61" s="44" t="s">
-        <v>225</v>
       </c>
       <c r="J61" s="43"/>
       <c r="K61" s="29"/>
@@ -3678,10 +3685,10 @@
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B63" s="39" t="s">
+        <v>225</v>
+      </c>
+      <c r="C63" s="40" t="s">
         <v>226</v>
-      </c>
-      <c r="C63" s="40" t="s">
-        <v>227</v>
       </c>
       <c r="D63" s="29"/>
       <c r="E63" s="29"/>
@@ -3698,7 +3705,7 @@
         <v>1</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D64" s="29"/>
       <c r="E64" s="30"/>
@@ -3707,13 +3714,13 @@
         <v></v>
       </c>
       <c r="G64" s="44" t="s">
+        <v>228</v>
+      </c>
+      <c r="H64" s="44" t="s">
         <v>229</v>
       </c>
-      <c r="H64" s="44" t="s">
+      <c r="I64" s="44" t="s">
         <v>230</v>
-      </c>
-      <c r="I64" s="44" t="s">
-        <v>231</v>
       </c>
       <c r="J64" s="43"/>
       <c r="K64" s="29"/>
@@ -3724,7 +3731,7 @@
         <v>2</v>
       </c>
       <c r="C65" s="28" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D65" s="29"/>
       <c r="E65" s="30"/>
@@ -3733,13 +3740,13 @@
         <v></v>
       </c>
       <c r="G65" s="44" t="s">
+        <v>232</v>
+      </c>
+      <c r="H65" s="44" t="s">
         <v>233</v>
       </c>
-      <c r="H65" s="44" t="s">
+      <c r="I65" s="44" t="s">
         <v>234</v>
-      </c>
-      <c r="I65" s="44" t="s">
-        <v>235</v>
       </c>
       <c r="J65" s="43"/>
       <c r="K65" s="29"/>
@@ -3750,7 +3757,7 @@
         <v>3</v>
       </c>
       <c r="C66" s="45" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D66" s="29"/>
       <c r="E66" s="30"/>
@@ -3759,13 +3766,13 @@
         <v></v>
       </c>
       <c r="G66" s="44" t="s">
+        <v>236</v>
+      </c>
+      <c r="H66" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="H66" s="44" t="s">
+      <c r="I66" s="44" t="s">
         <v>238</v>
-      </c>
-      <c r="I66" s="44" t="s">
-        <v>239</v>
       </c>
       <c r="J66" s="43"/>
       <c r="K66" s="29"/>
@@ -3776,7 +3783,7 @@
         <v>4</v>
       </c>
       <c r="C67" s="45" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="30"/>
@@ -3785,13 +3792,13 @@
         <v></v>
       </c>
       <c r="G67" s="44" t="s">
+        <v>240</v>
+      </c>
+      <c r="H67" s="44" t="s">
         <v>241</v>
       </c>
-      <c r="H67" s="44" t="s">
+      <c r="I67" s="44" t="s">
         <v>242</v>
-      </c>
-      <c r="I67" s="44" t="s">
-        <v>243</v>
       </c>
       <c r="J67" s="43"/>
       <c r="K67" s="29"/>
@@ -3802,7 +3809,7 @@
         <v>5</v>
       </c>
       <c r="C68" s="45" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D68" s="29"/>
       <c r="E68" s="30"/>
@@ -3811,13 +3818,13 @@
         <v></v>
       </c>
       <c r="G68" s="44" t="s">
+        <v>244</v>
+      </c>
+      <c r="H68" s="44" t="s">
         <v>245</v>
       </c>
-      <c r="H68" s="44" t="s">
+      <c r="I68" s="44" t="s">
         <v>246</v>
-      </c>
-      <c r="I68" s="44" t="s">
-        <v>247</v>
       </c>
       <c r="J68" s="43"/>
       <c r="K68" s="29"/>
@@ -3828,7 +3835,7 @@
         <v>6</v>
       </c>
       <c r="C69" s="45" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D69" s="29"/>
       <c r="E69" s="30"/>
@@ -3837,13 +3844,13 @@
         <v></v>
       </c>
       <c r="G69" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="H69" s="44" t="s">
         <v>249</v>
       </c>
-      <c r="H69" s="44" t="s">
+      <c r="I69" s="44" t="s">
         <v>250</v>
-      </c>
-      <c r="I69" s="44" t="s">
-        <v>251</v>
       </c>
       <c r="J69" s="43"/>
       <c r="K69" s="29"/>
@@ -3854,7 +3861,7 @@
         <v>7</v>
       </c>
       <c r="C70" s="45" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D70" s="29"/>
       <c r="E70" s="30"/>
@@ -3863,13 +3870,13 @@
         <v></v>
       </c>
       <c r="G70" s="44" t="s">
+        <v>252</v>
+      </c>
+      <c r="H70" s="44" t="s">
         <v>253</v>
       </c>
-      <c r="H70" s="44" t="s">
+      <c r="I70" s="44" t="s">
         <v>254</v>
-      </c>
-      <c r="I70" s="44" t="s">
-        <v>255</v>
       </c>
       <c r="J70" s="43"/>
       <c r="K70" s="29"/>
@@ -3880,7 +3887,7 @@
         <v>8</v>
       </c>
       <c r="C71" s="45" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D71" s="29"/>
       <c r="E71" s="30"/>
@@ -3889,13 +3896,13 @@
         <v></v>
       </c>
       <c r="G71" s="47" t="s">
+        <v>256</v>
+      </c>
+      <c r="H71" s="47" t="s">
         <v>257</v>
       </c>
-      <c r="H71" s="47" t="s">
+      <c r="I71" s="47" t="s">
         <v>258</v>
-      </c>
-      <c r="I71" s="47" t="s">
-        <v>259</v>
       </c>
       <c r="J71" s="43"/>
       <c r="K71" s="29"/>
@@ -3916,10 +3923,10 @@
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B73" s="39" t="s">
+        <v>259</v>
+      </c>
+      <c r="C73" s="40" t="s">
         <v>260</v>
-      </c>
-      <c r="C73" s="40" t="s">
-        <v>261</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="29"/>
@@ -3935,23 +3942,23 @@
       <c r="B74" s="32">
         <v>1</v>
       </c>
-      <c r="C74" s="61" t="s">
-        <v>262</v>
-      </c>
-      <c r="D74" s="61"/>
-      <c r="E74" s="61"/>
-      <c r="F74" s="59" t="str">
+      <c r="C74" s="70" t="s">
+        <v>261</v>
+      </c>
+      <c r="D74" s="70"/>
+      <c r="E74" s="70"/>
+      <c r="F74" s="71" t="str">
         <f>IF(OR(H74&lt;&gt;"",I74&lt;&gt;""), "", "")</f>
         <v></v>
       </c>
-      <c r="G74" s="62" t="s">
+      <c r="G74" s="72" t="s">
+        <v>262</v>
+      </c>
+      <c r="H74" s="72" t="s">
         <v>263</v>
       </c>
-      <c r="H74" s="62" t="s">
+      <c r="I74" s="72" t="s">
         <v>264</v>
-      </c>
-      <c r="I74" s="62" t="s">
-        <v>265</v>
       </c>
       <c r="J74" s="48"/>
       <c r="K74" s="19"/>
@@ -3959,18 +3966,18 @@
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B75" s="49"/>
-      <c r="C75" s="61"/>
-      <c r="D75" s="61"/>
-      <c r="E75" s="61"/>
-      <c r="F75" s="59"/>
-      <c r="G75" s="62" t="s">
+      <c r="C75" s="70"/>
+      <c r="D75" s="70"/>
+      <c r="E75" s="70"/>
+      <c r="F75" s="71"/>
+      <c r="G75" s="72" t="s">
+        <v>262</v>
+      </c>
+      <c r="H75" s="72" t="s">
         <v>263</v>
       </c>
-      <c r="H75" s="62" t="s">
+      <c r="I75" s="72" t="s">
         <v>264</v>
-      </c>
-      <c r="I75" s="62" t="s">
-        <v>265</v>
       </c>
       <c r="J75" s="22"/>
       <c r="K75" s="23"/>
@@ -3980,23 +3987,23 @@
       <c r="B76" s="32">
         <v>2</v>
       </c>
-      <c r="C76" s="61" t="s">
-        <v>266</v>
-      </c>
-      <c r="D76" s="61"/>
-      <c r="E76" s="61"/>
-      <c r="F76" s="59" t="str">
+      <c r="C76" s="70" t="s">
+        <v>265</v>
+      </c>
+      <c r="D76" s="70"/>
+      <c r="E76" s="70"/>
+      <c r="F76" s="71" t="str">
         <f>IF(OR(H76&lt;&gt;"",I76&lt;&gt;""), "", "")</f>
         <v></v>
       </c>
-      <c r="G76" s="62" t="s">
+      <c r="G76" s="72" t="s">
+        <v>266</v>
+      </c>
+      <c r="H76" s="72" t="s">
         <v>267</v>
       </c>
-      <c r="H76" s="62" t="s">
+      <c r="I76" s="72" t="s">
         <v>268</v>
-      </c>
-      <c r="I76" s="62" t="s">
-        <v>269</v>
       </c>
       <c r="J76" s="48"/>
       <c r="K76" s="19"/>
@@ -4004,13 +4011,13 @@
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B77" s="49"/>
-      <c r="C77" s="61"/>
-      <c r="D77" s="61"/>
-      <c r="E77" s="61"/>
-      <c r="F77" s="59"/>
-      <c r="G77" s="62"/>
-      <c r="H77" s="62"/>
-      <c r="I77" s="62"/>
+      <c r="C77" s="70"/>
+      <c r="D77" s="70"/>
+      <c r="E77" s="70"/>
+      <c r="F77" s="71"/>
+      <c r="G77" s="72"/>
+      <c r="H77" s="72"/>
+      <c r="I77" s="72"/>
       <c r="J77" s="22"/>
       <c r="K77" s="23"/>
       <c r="L77" s="24"/>
@@ -4043,10 +4050,10 @@
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B80" s="39" t="s">
+        <v>269</v>
+      </c>
+      <c r="C80" s="40" t="s">
         <v>270</v>
-      </c>
-      <c r="C80" s="40" t="s">
-        <v>271</v>
       </c>
       <c r="D80" s="29"/>
       <c r="E80" s="29"/>
@@ -4062,23 +4069,23 @@
       <c r="B81" s="32">
         <v>1</v>
       </c>
-      <c r="C81" s="58" t="s">
-        <v>272</v>
-      </c>
-      <c r="D81" s="58"/>
-      <c r="E81" s="58"/>
-      <c r="F81" s="59" t="str">
+      <c r="C81" s="74" t="s">
+        <v>271</v>
+      </c>
+      <c r="D81" s="74"/>
+      <c r="E81" s="74"/>
+      <c r="F81" s="71" t="str">
         <f>IF(OR(H81&lt;&gt;"",I81&lt;&gt;""), "", "")</f>
         <v></v>
       </c>
-      <c r="G81" s="60" t="s">
+      <c r="G81" s="73" t="s">
+        <v>272</v>
+      </c>
+      <c r="H81" s="73" t="s">
         <v>273</v>
       </c>
-      <c r="H81" s="60" t="s">
+      <c r="I81" s="73" t="s">
         <v>274</v>
-      </c>
-      <c r="I81" s="60" t="s">
-        <v>275</v>
       </c>
       <c r="J81" s="48"/>
       <c r="K81" s="19"/>
@@ -4086,13 +4093,13 @@
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B82" s="49"/>
-      <c r="C82" s="58"/>
-      <c r="D82" s="58"/>
-      <c r="E82" s="58"/>
-      <c r="F82" s="59"/>
-      <c r="G82" s="60"/>
-      <c r="H82" s="60"/>
-      <c r="I82" s="60"/>
+      <c r="C82" s="74"/>
+      <c r="D82" s="74"/>
+      <c r="E82" s="74"/>
+      <c r="F82" s="71"/>
+      <c r="G82" s="73"/>
+      <c r="H82" s="73"/>
+      <c r="I82" s="73"/>
       <c r="J82" s="22"/>
       <c r="K82" s="23"/>
       <c r="L82" s="24"/>
@@ -4102,7 +4109,7 @@
         <v>2</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D83" s="29"/>
       <c r="E83" s="30"/>
@@ -4111,13 +4118,13 @@
         <v></v>
       </c>
       <c r="G83" s="44" t="s">
+        <v>276</v>
+      </c>
+      <c r="H83" s="44" t="s">
         <v>277</v>
       </c>
-      <c r="H83" s="44" t="s">
+      <c r="I83" s="42" t="s">
         <v>278</v>
-      </c>
-      <c r="I83" s="42" t="s">
-        <v>279</v>
       </c>
       <c r="J83" s="28"/>
       <c r="K83" s="29"/>
@@ -4128,7 +4135,7 @@
         <v>3</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D84" s="29"/>
       <c r="E84" s="30"/>
@@ -4137,13 +4144,13 @@
         <v></v>
       </c>
       <c r="G84" s="44" t="s">
+        <v>280</v>
+      </c>
+      <c r="H84" s="44" t="s">
         <v>281</v>
       </c>
-      <c r="H84" s="44" t="s">
+      <c r="I84" s="44" t="s">
         <v>282</v>
-      </c>
-      <c r="I84" s="44" t="s">
-        <v>283</v>
       </c>
       <c r="J84" s="28"/>
       <c r="K84" s="29"/>
@@ -4154,7 +4161,7 @@
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B86" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C86" s="19"/>
       <c r="D86" s="19"/>
@@ -4233,12 +4240,12 @@
       <c r="L91" s="24"/>
     </row>
     <row r="93" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B93" s="54" t="s">
-        <v>83</v>
-      </c>
-      <c r="C93" s="54"/>
-      <c r="D93" s="54"/>
-      <c r="E93" s="54"/>
+      <c r="B93" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="C93" s="56"/>
+      <c r="D93" s="56"/>
+      <c r="E93" s="56"/>
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B94" s="3"/>
@@ -4259,15 +4266,50 @@
       <c r="E97" s="23"/>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B98" s="54" t="s">
-        <v>84</v>
-      </c>
-      <c r="C98" s="54"/>
-      <c r="D98" s="54"/>
-      <c r="E98" s="54"/>
+      <c r="B98" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="C98" s="56"/>
+      <c r="D98" s="56"/>
+      <c r="E98" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="B93:E93"/>
+    <mergeCell ref="B98:E98"/>
+    <mergeCell ref="C81:E82"/>
+    <mergeCell ref="F81:F82"/>
+    <mergeCell ref="G81:G82"/>
+    <mergeCell ref="H81:H82"/>
+    <mergeCell ref="I81:I82"/>
+    <mergeCell ref="C76:E77"/>
+    <mergeCell ref="F76:F77"/>
+    <mergeCell ref="G76:G77"/>
+    <mergeCell ref="H76:H77"/>
+    <mergeCell ref="I76:I77"/>
+    <mergeCell ref="C74:E75"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="G74:G75"/>
+    <mergeCell ref="H74:H75"/>
+    <mergeCell ref="I74:I75"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:E38"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="J36:L38"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:L31"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C18:L18"/>
@@ -4278,41 +4320,6 @@
     <mergeCell ref="J27:L29"/>
     <mergeCell ref="F28:G29"/>
     <mergeCell ref="H28:I29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C36:E38"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="J36:L38"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="C74:E75"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="G74:G75"/>
-    <mergeCell ref="H74:H75"/>
-    <mergeCell ref="I74:I75"/>
-    <mergeCell ref="H81:H82"/>
-    <mergeCell ref="I81:I82"/>
-    <mergeCell ref="C76:E77"/>
-    <mergeCell ref="F76:F77"/>
-    <mergeCell ref="G76:G77"/>
-    <mergeCell ref="H76:H77"/>
-    <mergeCell ref="I76:I77"/>
-    <mergeCell ref="B93:E93"/>
-    <mergeCell ref="B98:E98"/>
-    <mergeCell ref="C81:E82"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="G81:G82"/>
   </mergeCells>
   <pageMargins left="0.37013888888888902" right="0.25972222222222202" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>